<commit_message>
everything works and tesi updated on transformer_simple 50-80
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\Thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C03FEFC7-F50A-4320-B6FF-293D1304613C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE9A64C9-C3C6-4323-9A35-8978D00EC92A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="210" yWindow="300" windowWidth="14400" windowHeight="7360" xr2:uid="{AA462D55-4BD8-4A3F-90EA-FEFBCFBC68BD}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="10">
   <si>
     <t>RMSE</t>
   </si>
@@ -44,18 +44,6 @@
     <t>models</t>
   </si>
   <si>
-    <t>FCNN</t>
-  </si>
-  <si>
-    <t>CNN</t>
-  </si>
-  <si>
-    <t>LSTM</t>
-  </si>
-  <si>
-    <t>transformer</t>
-  </si>
-  <si>
     <t>EOG</t>
   </si>
   <si>
@@ -72,6 +60,12 @@
   </si>
   <si>
     <t>SSIM</t>
+  </si>
+  <si>
+    <t>transformer simple</t>
+  </si>
+  <si>
+    <t>epochs</t>
   </si>
 </sst>
 </file>
@@ -159,10 +153,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -171,13 +164,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -495,120 +488,124 @@
   <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="C3" sqref="C3:F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="14.7265625" customWidth="1"/>
-    <col min="3" max="3" width="10.26953125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="16" customWidth="1"/>
+    <col min="3" max="3" width="10.26953125" style="2" customWidth="1"/>
     <col min="4" max="6" width="10.26953125" customWidth="1"/>
-    <col min="7" max="7" width="10.26953125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="10.26953125" style="2" customWidth="1"/>
     <col min="8" max="10" width="10.26953125" customWidth="1"/>
-    <col min="11" max="11" width="10.26953125" style="3" customWidth="1"/>
+    <col min="11" max="11" width="10.26953125" style="2" customWidth="1"/>
     <col min="12" max="14" width="10.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="4" t="s">
+    <row r="1" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D1" s="7"/>
       <c r="E1" s="7"/>
       <c r="F1" s="7"/>
       <c r="G1" s="7" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="H1" s="7"/>
       <c r="I1" s="7"/>
       <c r="J1" s="7"/>
       <c r="K1" s="7" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="L1" s="7"/>
       <c r="M1" s="7"/>
       <c r="N1" s="7"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="C2" s="5" t="s">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" s="5" t="s">
+      <c r="D2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="H2" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="K2" s="5" t="s">
+      <c r="H2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="K2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="L2" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="M2" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="N2" s="6" t="s">
-        <v>11</v>
+      <c r="L2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A3" s="8"/>
+      <c r="A3" s="8">
+        <v>50</v>
+      </c>
       <c r="B3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="9">
-        <v>0.45123871999999998</v>
-      </c>
-      <c r="D3" s="9">
-        <v>0.89066731493418405</v>
-      </c>
-      <c r="E3" s="9">
-        <v>18.952606779644402</v>
-      </c>
-      <c r="F3" s="9">
-        <v>0.591182088845564</v>
-      </c>
-      <c r="G3" s="2"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
+        <v>8</v>
+      </c>
+      <c r="C3" s="6">
+        <v>0.70389461498114902</v>
+      </c>
+      <c r="D3" s="6">
+        <v>0.661825089833181</v>
+      </c>
+      <c r="E3" s="6">
+        <v>13.240868748151801</v>
+      </c>
+      <c r="F3" s="6">
+        <v>0.26438746185434397</v>
+      </c>
+      <c r="G3" s="1">
+        <v>0.52420581224005502</v>
+      </c>
+      <c r="H3" s="1">
+        <v>0.82352536484161898</v>
+      </c>
+      <c r="I3" s="1">
+        <v>16.197356524641201</v>
+      </c>
+      <c r="J3" s="1">
+        <v>0.44115773940263903</v>
+      </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" s="8"/>
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" s="8"/>
-      <c r="B5" t="s">
-        <v>4</v>
-      </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" s="8"/>
-      <c r="B6" t="s">
-        <v>5</v>
-      </c>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
transformer simple 50 80 working
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\Thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE9A64C9-C3C6-4323-9A35-8978D00EC92A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1203E05-76F2-48FB-B422-575A26D762E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="210" yWindow="300" windowWidth="14400" windowHeight="7360" xr2:uid="{AA462D55-4BD8-4A3F-90EA-FEFBCFBC68BD}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="11">
   <si>
     <t>RMSE</t>
   </si>
@@ -66,6 +66,9 @@
   </si>
   <si>
     <t>epochs</t>
+  </si>
+  <si>
+    <t>80/50</t>
   </si>
 </sst>
 </file>
@@ -168,9 +171,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -488,7 +489,7 @@
   <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:F3"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -599,7 +600,36 @@
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A4" s="8"/>
+      <c r="A4" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0.60591153580771195</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0.76717203368462905</v>
+      </c>
+      <c r="E4" s="1">
+        <v>14.4484940182891</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0.34216573947483497</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0.52420581224005502</v>
+      </c>
+      <c r="H4" s="1">
+        <v>0.82352536484161898</v>
+      </c>
+      <c r="I4" s="1">
+        <v>16.197356524641201</v>
+      </c>
+      <c r="J4" s="1">
+        <v>0.44115773940263903</v>
+      </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" s="8"/>
@@ -608,11 +638,10 @@
       <c r="A6" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="3">
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="G1:J1"/>
     <mergeCell ref="K1:N1"/>
-    <mergeCell ref="A3:A6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
model positional transformer working 80 60 tesi not updated
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\Thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1203E05-76F2-48FB-B422-575A26D762E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{575E2914-8F5D-469A-90C8-B9DBC1BD9A5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="210" yWindow="300" windowWidth="14400" windowHeight="7360" xr2:uid="{AA462D55-4BD8-4A3F-90EA-FEFBCFBC68BD}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="13">
   <si>
     <t>RMSE</t>
   </si>
@@ -69,13 +69,19 @@
   </si>
   <si>
     <t>80/50</t>
+  </si>
+  <si>
+    <t>positional encoding</t>
+  </si>
+  <si>
+    <t>80/60</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -91,6 +97,12 @@
     <font>
       <sz val="7"/>
       <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FF3C4043"/>
+      <name val="Roboto Mono"/>
       <family val="3"/>
     </font>
   </fonts>
@@ -168,10 +180,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -486,10 +500,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A05F00A2-C0AD-44B1-A299-D3D330C4130B}">
-  <dimension ref="A1:N6"/>
+  <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -507,24 +521,24 @@
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7" t="s">
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7" t="s">
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7"/>
-      <c r="N1" s="7"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
@@ -568,7 +582,7 @@
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A3" s="8">
+      <c r="A3">
         <v>50</v>
       </c>
       <c r="B3" t="s">
@@ -600,7 +614,7 @@
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A4" s="8" t="s">
+      <c r="A4" t="s">
         <v>10</v>
       </c>
       <c r="B4" t="s">
@@ -632,10 +646,36 @@
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A5" s="8"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A6" s="8"/>
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="7">
+        <v>0.37198085137525</v>
+      </c>
+      <c r="D5" s="7">
+        <v>0.91844895957392003</v>
+      </c>
+      <c r="E5" s="7">
+        <v>19.101399091727401</v>
+      </c>
+      <c r="F5" s="7">
+        <v>0.60977840904262803</v>
+      </c>
+      <c r="G5" s="7">
+        <v>0.53484263251855302</v>
+      </c>
+      <c r="H5" s="7">
+        <v>0.82396410053204105</v>
+      </c>
+      <c r="I5" s="7">
+        <v>16.138007493524199</v>
+      </c>
+      <c r="J5" s="7">
+        <v>0.44981908248031299</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>